<commit_message>
Revert back properties dictionaries
</commit_message>
<xml_diff>
--- a/Codelist Excel Files and Conversion Templates to XML/measurand.xlsx
+++ b/Codelist Excel Files and Conversion Templates to XML/measurand.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10511"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rosscutts/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dponti/GitHub/def/Codelist Excel Files and Conversion Templates to XML/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7275485-4214-6745-B76F-D3DE218A157A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA570B61-8B73-054B-AE6C-DD5888B23373}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9200" yWindow="2460" windowWidth="39400" windowHeight="24940" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9200" yWindow="3280" windowWidth="39400" windowHeight="24940" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DictionaryName" sheetId="3" r:id="rId1"/>
@@ -1956,7 +1956,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -2032,8 +2032,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView topLeftCell="A17" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B37" sqref="B27:B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2647,7 +2647,7 @@
       </c>
       <c r="G27" s="11"/>
     </row>
-    <row r="28" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="str">
         <f>IF(ISNA(VLOOKUP(B28,AssociatedElements!B$2:B2871,1,FALSE)),"Not used","")</f>
         <v/>
@@ -2665,7 +2665,7 @@
         <v>1</v>
       </c>
       <c r="F28" s="15" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="G28" s="11"/>
     </row>

</xml_diff>

<commit_message>
Update properties and measurand dictionaries
</commit_message>
<xml_diff>
--- a/Codelist Excel Files and Conversion Templates to XML/measurand.xlsx
+++ b/Codelist Excel Files and Conversion Templates to XML/measurand.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10511"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10824"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dponti/GitHub/def/Codelist Excel Files and Conversion Templates to XML/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA570B61-8B73-054B-AE6C-DD5888B23373}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00F108C6-BB4F-D04A-9911-CD2B0959E7A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9200" yWindow="3280" windowWidth="39400" windowHeight="24940" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="60300" yWindow="660" windowWidth="38100" windowHeight="19560" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DictionaryName" sheetId="3" r:id="rId1"/>
@@ -1956,7 +1956,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -2032,8 +2032,12 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B37" sqref="B27:B37"/>
+    <sheetView topLeftCell="A21" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane xSplit="1" ySplit="11" topLeftCell="B32" activePane="bottomRight" state="frozen"/>
+      <selection activeCell="A21" sqref="A21"/>
+      <selection pane="topRight" activeCell="B21" sqref="B21"/>
+      <selection pane="bottomLeft" activeCell="A32" sqref="A32"/>
+      <selection pane="bottomRight" activeCell="C21" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2877,7 +2881,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C29" sqref="C29"/>
     </sheetView>

</xml_diff>